<commit_message>
Added Year ID to UserSettings Updated queries to use UserSettings.YearId Added Injection Prevention to questionnaires to prevent changing of querystrings Header changes to put teacher name or Child EDI ID on top of forms
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Translation.xlsx
+++ b/EDI/Web/wwwroot/Upload/Translation.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andre\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>English</t>
   </si>
@@ -74,12 +81,6 @@
     <t>Tableau de bord</t>
   </si>
   <si>
-    <t>Dashboard for Teacher</t>
-  </si>
-  <si>
-    <t>Tableau de bord pour l'enseignant</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -246,13 +247,31 @@
   </si>
   <si>
     <t>An</t>
+  </si>
+  <si>
+    <t>Administrator Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord administrateur</t>
+  </si>
+  <si>
+    <t>Tableau de bord des enseignants</t>
+  </si>
+  <si>
+    <t>Teacher Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord du coordinateur</t>
+  </si>
+  <si>
+    <t>Coordinator Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
@@ -268,6 +287,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,6 +324,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -313,6 +339,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -327,373 +354,669 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="GridTranslationcolumn1" xfId="1"/>
     <cellStyle name="GridTranslationcolumn2" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.284285714285714" customWidth="1"/>
-    <col min="2" max="2" width="4.284285714285714" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s" s="4">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="4">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s" s="2">
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s" s="2">
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s" s="2">
+    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s" s="2">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s" s="2">
+    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s" s="2">
+    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s" s="2">
+    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s" s="2">
+    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s" s="2">
+    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s" s="3">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s" s="2">
+    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s" s="2">
+    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s" s="3">
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s" s="2">
+    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s" s="2">
+    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s" s="2">
+    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s" s="2">
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s" s="3">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s" s="2">
+    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s" s="2">
+    </row>
+    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s" s="2">
+    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s" s="3">
+      <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s" s="2">
+    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s" s="2">
+    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s" s="3">
+      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s" s="2">
+    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s" s="2">
+    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s" s="3">
+      <c r="B29" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s" s="2">
+    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s" s="3">
+      <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s" s="2">
+    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s" s="3">
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s" s="2">
+    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s" s="3">
+      <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s" s="2">
+    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s" s="3">
+      <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s" s="2">
+    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s" s="3">
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s" s="2">
+      <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s" s="2">
+    </row>
+    <row r="36" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s" s="3">
+      <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s" s="2">
+    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s" s="3">
+      <c r="B37" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s" s="2">
+    <row r="38" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s" s="3">
+      <c r="B38" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s" s="2">
+    <row r="39" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s" s="3">
+      <c r="B39" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s" s="2">
+    <row r="40" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s" s="3">
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s" s="2">
+    <row r="41" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s" s="3">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s" s="3">
-        <v>77</v>
-      </c>
+    <row r="42" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Questionnaire Updated Round 1
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Translation.xlsx
+++ b/EDI/Web/wwwroot/Upload/Translation.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andre\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>English</t>
   </si>
@@ -74,12 +81,6 @@
     <t>Tableau de bord</t>
   </si>
   <si>
-    <t>Dashboard for Teacher</t>
-  </si>
-  <si>
-    <t>Tableau de bord pour l'enseignant</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -246,13 +247,31 @@
   </si>
   <si>
     <t>An</t>
+  </si>
+  <si>
+    <t>Administrator Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord administrateur</t>
+  </si>
+  <si>
+    <t>Tableau de bord des enseignants</t>
+  </si>
+  <si>
+    <t>Teacher Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord du coordinateur</t>
+  </si>
+  <si>
+    <t>Coordinator Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
@@ -268,6 +287,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,6 +324,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -313,6 +339,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -327,373 +354,669 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="GridTranslationcolumn1" xfId="1"/>
     <cellStyle name="GridTranslationcolumn2" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.284285714285714" customWidth="1"/>
-    <col min="2" max="2" width="4.284285714285714" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s" s="4">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="4">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s" s="2">
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s" s="2">
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s" s="2">
+    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s" s="2">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s" s="2">
+    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s" s="2">
+    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s" s="2">
+    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s" s="2">
+    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s" s="2">
+    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s" s="3">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s" s="2">
+    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s" s="2">
+    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s" s="3">
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s" s="2">
+    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s" s="2">
+    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s" s="2">
+    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s" s="2">
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s" s="3">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s" s="2">
+    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s" s="2">
+    </row>
+    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s" s="2">
+    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s" s="3">
+      <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s" s="2">
+    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s" s="2">
+    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s" s="3">
+      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s" s="2">
+    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s" s="2">
+    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s" s="3">
+      <c r="B29" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s" s="2">
+    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s" s="3">
+      <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s" s="2">
+    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s" s="3">
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s" s="2">
+    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s" s="3">
+      <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s" s="2">
+    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s" s="3">
+      <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s" s="2">
+    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s" s="3">
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s" s="2">
+      <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s" s="2">
+    </row>
+    <row r="36" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s" s="3">
+      <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s" s="2">
+    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s" s="3">
+      <c r="B37" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s" s="2">
+    <row r="38" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s" s="3">
+      <c r="B38" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s" s="2">
+    <row r="39" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s" s="3">
+      <c r="B39" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s" s="2">
+    <row r="40" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s" s="3">
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s" s="2">
+    <row r="41" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s" s="3">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s" s="3">
-        <v>77</v>
-      </c>
+    <row r="42" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validation Checks Removed Toast on Navigation
</commit_message>
<xml_diff>
--- a/EDI/Web/wwwroot/Upload/Translation.xlsx
+++ b/EDI/Web/wwwroot/Upload/Translation.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andre\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>English</t>
   </si>
@@ -74,12 +81,6 @@
     <t>Tableau de bord</t>
   </si>
   <si>
-    <t>Dashboard for Teacher</t>
-  </si>
-  <si>
-    <t>Tableau de bord pour l'enseignant</t>
-  </si>
-  <si>
     <t>Date of Birth</t>
   </si>
   <si>
@@ -246,13 +247,31 @@
   </si>
   <si>
     <t>An</t>
+  </si>
+  <si>
+    <t>Administrator Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord administrateur</t>
+  </si>
+  <si>
+    <t>Tableau de bord des enseignants</t>
+  </si>
+  <si>
+    <t>Teacher Dashboard</t>
+  </si>
+  <si>
+    <t>Tableau de bord du coordinateur</t>
+  </si>
+  <si>
+    <t>Coordinator Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
@@ -268,6 +287,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,6 +324,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -313,6 +339,7 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -327,373 +354,669 @@
       <bottom style="thin">
         <color rgb="FFE0E0E0"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="GridTranslationcolumn1" xfId="1"/>
     <cellStyle name="GridTranslationcolumn2" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.284285714285714" customWidth="1"/>
-    <col min="2" max="2" width="4.284285714285714" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s" s="4">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="4">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s" s="2">
+    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s" s="2">
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s" s="2">
+    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s" s="2">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s" s="2">
+    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s" s="2">
+    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s" s="2">
+    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s" s="2">
+    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s" s="2">
+    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s" s="3">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s" s="2">
+    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s" s="2">
+    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s" s="3">
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s" s="2">
+    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s" s="2">
+    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s" s="2">
+    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s" s="2">
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s" s="3">
+      <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s" s="2">
+    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s" s="2">
+    </row>
+    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s" s="2">
+    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s" s="3">
+      <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s" s="2">
+    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s" s="2">
+    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s" s="3">
+      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s" s="2">
+    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s" s="2">
+    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s" s="3">
+      <c r="B29" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s" s="2">
+    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s" s="3">
+      <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s" s="2">
+    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s" s="3">
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s" s="2">
+    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s" s="3">
+      <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s" s="2">
+    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s" s="3">
+      <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s" s="2">
+    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s" s="3">
+      <c r="B34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s" s="2">
+      <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s" s="3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s" s="2">
+    </row>
+    <row r="36" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s" s="3">
+      <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s" s="2">
+    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s" s="3">
+      <c r="B37" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s" s="2">
+    <row r="38" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s" s="3">
+      <c r="B38" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s" s="2">
+    <row r="39" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s" s="3">
+      <c r="B39" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s" s="2">
+    <row r="40" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s" s="3">
+      <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s" s="2">
+    <row r="41" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s" s="3">
+      <c r="B41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s" s="3">
-        <v>77</v>
-      </c>
+    <row r="42" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>